<commit_message>
Refactor frontend crop and farm components
Removed unused CropDetailPage and FarmDetail_Simple components, updated crop and farm related components for improved structure, and added a new useServerStatus hook and crop.csv data file. Also updated .vs and obj files as part of development environment changes.
</commit_message>
<xml_diff>
--- a/Task Excel Worksheet.xlsx
+++ b/Task Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_CODES\.NET_Project\AgroSmart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B37E4E-FDC0-46B0-AA20-25BB62AB8424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F48563-4148-48A4-B532-DD54CDB132DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,37 +25,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Sr.</t>
   </si>
   <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Timing or Planning For Features</t>
-  </si>
-  <si>
-    <t>Extra or Add on</t>
-  </si>
-  <si>
-    <t>Regular tasks</t>
-  </si>
-  <si>
-    <t>Addon Learning</t>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Complete AgroSmart Project</t>
+  </si>
+  <si>
+    <t>AgroSmart</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Fetures</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>API Creation Of All Table</t>
+  </si>
+  <si>
+    <t>crud DDL</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Complatted</t>
+  </si>
+  <si>
+    <t>Complete Crud And Filter on crop table</t>
+  </si>
+  <si>
+    <t>perform crud and filter</t>
+  </si>
+  <si>
+    <t>Compalted</t>
+  </si>
+  <si>
+    <t>Complete Crud And Filter on Farm table</t>
+  </si>
+  <si>
+    <t>Complete Crud And Filter on Field table</t>
+  </si>
+  <si>
+    <t>Link Farm Field Crop with FieldWiseCrop table</t>
+  </si>
+  <si>
+    <t>Weather CRUD and fetching from live api</t>
+  </si>
+  <si>
+    <t>Implement Schdeule</t>
+  </si>
+  <si>
+    <t>Implement Sensors</t>
+  </si>
+  <si>
+    <t>Auto get Sensor Readings</t>
+  </si>
+  <si>
+    <t>Work on login and user profile</t>
+  </si>
+  <si>
+    <t>Work on Dashboard</t>
+  </si>
+  <si>
+    <t>work on SmartInsights</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Algerian"/>
+      <family val="5"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Algerian"/>
+      <family val="5"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -74,12 +160,137 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,59 +571,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="J4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6">
+        <v>45869</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6">
+        <v>45869</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6">
+        <v>45869</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6">
+        <v>45869</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="6">
+        <v>45874</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6">
+        <v>45879</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="6">
+        <v>45884</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6">
+        <v>45894</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6">
+        <v>45899</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6">
+        <v>45905</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>